<commit_message>
fix bugs in openspace logic
</commit_message>
<xml_diff>
--- a/colleagues.xlsx
+++ b/colleagues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\38050\projects\openspace-organizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F4360A-B212-41E8-A457-862E33836459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06A0689-BD72-44D9-8B3E-7666D978F622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4B228CC-19D1-426F-8E09-8625E5804A52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Sebastiaan</t>
+  </si>
+  <si>
+    <t>Oleh</t>
   </si>
 </sst>
 </file>
@@ -169,9 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD135161-1B0C-429A-AC78-6856D543B384}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,6 +631,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>